<commit_message>
kosmetické úpravy při zachování funkce
</commit_message>
<xml_diff>
--- a/data-raw/vzorek.xlsx
+++ b/data-raw/vzorek.xlsx
@@ -403,7 +403,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>hnízdiště &lt;i&gt;&lt;a href = "https://cs.wikipedia.org/wiki/%C4%8C%C3%A1p_b%C3%ADl%C3%BD"&gt;Ciconia ciconia L. 1758&lt;/a&gt;&lt;/i&gt;</t>
+          <t>hnízdiště &lt;i&gt;&lt;a href = "https://cs.wikipedia.org/wiki/%C4%8C%C3%A1p_b%C3%ADl%C3%BD"&gt;Ciconia ciconia L.&lt;/a&gt;&lt;/i&gt;</t>
         </is>
       </c>
     </row>
@@ -449,7 +449,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>akademie &lt;i&gt;&lt;a href="https://cs.wikipedia.org/wiki/Straka_obecn%C3%A1"&gt;Pica pica L. 1758&lt;/a&gt;&lt;/i&gt;</t>
+          <t>zimoviště &lt;i&gt;&lt;a href="https://cs.wikipedia.org/wiki/Straka_obecn%C3%A1"&gt;Pica pica L.&lt;/a&gt;&lt;/i&gt;</t>
         </is>
       </c>
     </row>

</xml_diff>